<commit_message>
Names updated on valid employees sheet
</commit_message>
<xml_diff>
--- a/PaylocityBenefitsDashboard_V1/src/test/java/com/paylocitybenefitsdashboard/testData/Employees.xlsx
+++ b/PaylocityBenefitsDashboard_V1/src/test/java/com/paylocitybenefitsdashboard/testData/Employees.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="20100" windowHeight="8865" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="20835" windowHeight="4065"/>
   </bookViews>
   <sheets>
     <sheet name="employees-valid" sheetId="1" r:id="rId1"/>
     <sheet name="employees-updated" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <oleSize ref="A1:Q28"/>
+  <oleSize ref="A1:T12"/>
   <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
     <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="32">
   <si>
     <t>firstName</t>
   </si>
@@ -102,6 +102,30 @@
   </si>
   <si>
     <t>Kevin</t>
+  </si>
+  <si>
+    <t>Gandalf</t>
+  </si>
+  <si>
+    <t>Thegrey</t>
+  </si>
+  <si>
+    <t>Frodo</t>
+  </si>
+  <si>
+    <t>Baggins</t>
+  </si>
+  <si>
+    <t>Sam</t>
+  </si>
+  <si>
+    <t>Gamgee</t>
+  </si>
+  <si>
+    <t>Gollum</t>
+  </si>
+  <si>
+    <t>Smeagol</t>
   </si>
 </sst>
 </file>
@@ -452,7 +476,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -462,8 +486,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -486,10 +510,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>5</v>
@@ -497,32 +521,32 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>14</v>
@@ -539,7 +563,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>

</xml_diff>